<commit_message>
new changes has been made
</commit_message>
<xml_diff>
--- a/src/test/resources/Testdetails.xlsx
+++ b/src/test/resources/Testdetails.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>pincode</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>500072</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>7</t>
   </si>
 </sst>
 </file>
@@ -392,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -404,7 +410,7 @@
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -412,7 +418,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -420,7 +426,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -428,7 +434,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -436,7 +442,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -444,12 +450,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6">
-        <v>12</v>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>